<commit_message>
"Added DegreeRequirement and studenTerm and ApplicationDbContext"
</commit_message>
<xml_diff>
--- a/.net main.xlsx
+++ b/.net main.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S531495\Pictures\Team8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B91F224-4B1A-467F-9381-F90000F9B869}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70BAC61D-C090-4139-B3EA-1F73628EC9A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16410" windowHeight="7545" firstSheet="2" activeTab="5" xr2:uid="{2B808FE4-DBEC-4002-8F91-2211F4B4860B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16410" windowHeight="7545" xr2:uid="{2B808FE4-DBEC-4002-8F91-2211F4B4860B}"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="103">
   <si>
     <t>DegreeId</t>
   </si>
@@ -330,6 +330,21 @@
   </si>
   <si>
     <t>Sp24</t>
+  </si>
+  <si>
+    <t>opening</t>
+  </si>
+  <si>
+    <t>ending</t>
+  </si>
+  <si>
+    <t>str</t>
+  </si>
+  <si>
+    <t>new Degree{</t>
+  </si>
+  <si>
+    <t>},</t>
   </si>
 </sst>
 </file>
@@ -386,7 +401,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -395,6 +410,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -710,15 +727,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE356B96-A30F-42CD-ACEA-546DA74B1803}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="33.85546875" customWidth="1"/>
+    <col min="3" max="3" width="37.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -728,8 +751,17 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -739,8 +771,18 @@
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" s="9" t="str">
+        <f>D2&amp;$A$1&amp;"="&amp;A2&amp;E2</f>
+        <v>new Degree{DegreeId=1},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -750,8 +792,14 @@
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -761,8 +809,14 @@
       <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -771,6 +825,12 @@
       </c>
       <c r="C5" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2650,8 +2710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64FF7E25-1075-4403-8BC8-9554049F9FD7}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>